<commit_message>
major revisions with city of sonoma and other rw fixes
</commit_message>
<xml_diff>
--- a/Commercial_Freq_UseCode_Description.xlsx
+++ b/Commercial_Freq_UseCode_Description.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>GSA_Jurisdiction_Prelim</t>
   </si>
@@ -43,81 +43,78 @@
     <t>Dairy w/residence</t>
   </si>
   <si>
-    <t>City park/other rec facility</t>
+    <t>Miscellaneous state property</t>
+  </si>
+  <si>
+    <t>Sbe-valued utility</t>
+  </si>
+  <si>
+    <t>Light manuftg &amp; industrial</t>
+  </si>
+  <si>
+    <t>Warehousing yard</t>
+  </si>
+  <si>
+    <t>Auto and truck repair &amp; maint</t>
+  </si>
+  <si>
+    <t>Store w/res unit or units</t>
+  </si>
+  <si>
+    <t>Religious building</t>
+  </si>
+  <si>
+    <t>Specialty shop (tires, brakes)</t>
+  </si>
+  <si>
+    <t>Wholesale nursery</t>
+  </si>
+  <si>
+    <t>Chicken ranch w/residence</t>
+  </si>
+  <si>
+    <t>Cemetery</t>
+  </si>
+  <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>Com'l use/no other category</t>
+  </si>
+  <si>
+    <t>Retail nursery</t>
+  </si>
+  <si>
+    <t>Misc multiple use/none dominat</t>
+  </si>
+  <si>
+    <t>Light manufctrg &amp; warehousing</t>
+  </si>
+  <si>
+    <t>One story office building</t>
+  </si>
+  <si>
+    <t>Miscellaneous federal property</t>
+  </si>
+  <si>
+    <t>Mini-warehouse</t>
+  </si>
+  <si>
+    <t>Single story store</t>
+  </si>
+  <si>
+    <t>Used car lot</t>
+  </si>
+  <si>
+    <t>Single live/work unit</t>
   </si>
   <si>
     <t>Municipal utility property</t>
   </si>
   <si>
-    <t>Miscellaneous state property</t>
-  </si>
-  <si>
-    <t>Light manuftg &amp; industrial</t>
-  </si>
-  <si>
-    <t>Sbe-valued utility</t>
-  </si>
-  <si>
-    <t>Warehousing yard</t>
-  </si>
-  <si>
-    <t>Store w/res unit or units</t>
-  </si>
-  <si>
-    <t>Auto and truck repair &amp; maint</t>
-  </si>
-  <si>
-    <t>Specialty shop (tires, brakes)</t>
-  </si>
-  <si>
-    <t>Religious building</t>
-  </si>
-  <si>
-    <t>Wholesale nursery</t>
-  </si>
-  <si>
-    <t>Chicken ranch w/residence</t>
-  </si>
-  <si>
-    <t>Cemetery</t>
-  </si>
-  <si>
-    <t>Dairy</t>
-  </si>
-  <si>
-    <t>Retail nursery</t>
-  </si>
-  <si>
-    <t>Single story store</t>
-  </si>
-  <si>
-    <t>Com'l use/no other category</t>
-  </si>
-  <si>
-    <t>Light manufctrg &amp; warehousing</t>
-  </si>
-  <si>
-    <t>Misc multiple use/none dominat</t>
-  </si>
-  <si>
-    <t>Mini-warehouse</t>
-  </si>
-  <si>
-    <t>Used car lot</t>
-  </si>
-  <si>
-    <t>One story office building</t>
-  </si>
-  <si>
-    <t>Miscellaneous federal property</t>
-  </si>
-  <si>
     <t>Winery w/vineyards</t>
   </si>
   <si>
-    <t>Single live/work unit</t>
-  </si>
-  <si>
     <t>Two story office building</t>
   </si>
   <si>
@@ -136,271 +133,265 @@
     <t>Neighborhood shopping center</t>
   </si>
   <si>
+    <t>Other sales: trailers, mbh, rv</t>
+  </si>
+  <si>
     <t>Privately owned park</t>
   </si>
   <si>
     <t>Rest home</t>
   </si>
   <si>
-    <t>Other sales: trailers, mbh, rv</t>
+    <t>Retail lumber yard</t>
+  </si>
+  <si>
+    <t>Meat products</t>
+  </si>
+  <si>
+    <t>Home for handicapped (physical, mental, etc.)</t>
+  </si>
+  <si>
+    <t>Industr'l in no other category</t>
   </si>
   <si>
     <t>Club/lodge hall</t>
   </si>
   <si>
-    <t>City building</t>
-  </si>
-  <si>
-    <t>Home for handicapped (physical, mental, etc.)</t>
-  </si>
-  <si>
-    <t>Meat products</t>
-  </si>
-  <si>
-    <t>Retail lumber yard</t>
-  </si>
-  <si>
-    <t>Industr'l in no other category</t>
+    <t>Specialty lumber products</t>
+  </si>
+  <si>
+    <t>Multiple stores in 1 structure</t>
+  </si>
+  <si>
+    <t>Truck terminal</t>
+  </si>
+  <si>
+    <t>Restaurant</t>
+  </si>
+  <si>
+    <t>Veterinary hospitals</t>
+  </si>
+  <si>
+    <t>Horse ranch w/res</t>
+  </si>
+  <si>
+    <t>Winery with vineyards</t>
+  </si>
+  <si>
+    <t>Chicken ranch</t>
+  </si>
+  <si>
+    <t>Airport/private</t>
+  </si>
+  <si>
+    <t>Full service station</t>
+  </si>
+  <si>
+    <t>Auto sales w/o service center</t>
+  </si>
+  <si>
+    <t>18 hole public golf course</t>
+  </si>
+  <si>
+    <t>Misc multiple use/no dominate</t>
+  </si>
+  <si>
+    <t>County building</t>
+  </si>
+  <si>
+    <t>Recreational center</t>
   </si>
   <si>
     <t>Multiple combo/stores &amp; office</t>
   </si>
   <si>
-    <t>Multiple stores in 1 structure</t>
-  </si>
-  <si>
-    <t>Restaurant</t>
-  </si>
-  <si>
-    <t>Specialty lumber products</t>
-  </si>
-  <si>
-    <t>Truck terminal</t>
-  </si>
-  <si>
-    <t>Veterinary hospitals</t>
-  </si>
-  <si>
-    <t>18 hole public golf course</t>
-  </si>
-  <si>
-    <t>Winery with vineyards</t>
-  </si>
-  <si>
-    <t>Horse ranch w/res</t>
-  </si>
-  <si>
-    <t>Full service station</t>
-  </si>
-  <si>
-    <t>Chicken ranch</t>
-  </si>
-  <si>
-    <t>Auto sales w/o service center</t>
-  </si>
-  <si>
-    <t>Airport/private</t>
+    <t>Alternate use office bldgs</t>
+  </si>
+  <si>
+    <t>Fire district</t>
+  </si>
+  <si>
+    <t>Grocery store</t>
   </si>
   <si>
     <t>Horse ranch w/2 or more residences</t>
   </si>
   <si>
-    <t>Grocery store</t>
-  </si>
-  <si>
-    <t>Recreational center</t>
+    <t>Utility water company</t>
+  </si>
+  <si>
+    <t>Medical offices</t>
+  </si>
+  <si>
+    <t>Bulk plant</t>
+  </si>
+  <si>
+    <t>Sand &amp; gravel, shale</t>
+  </si>
+  <si>
+    <t>Industrial common area</t>
   </si>
   <si>
     <t>Other food processing plants</t>
   </si>
   <si>
-    <t>Sand &amp; gravel, shale</t>
-  </si>
-  <si>
-    <t>Fire district</t>
+    <t>Cocktail lounge bar</t>
+  </si>
+  <si>
+    <t>State pk/other recreation fac</t>
+  </si>
+  <si>
+    <t>Sand and gravel, shale</t>
   </si>
   <si>
     <t>Sfd converted to residential care facility</t>
   </si>
   <si>
-    <t>Bulk plant</t>
-  </si>
-  <si>
-    <t>Industrial common area</t>
-  </si>
-  <si>
-    <t>Misc multiple use/no dominate</t>
-  </si>
-  <si>
-    <t>Medical offices</t>
+    <t>Arcades &amp; amusement center</t>
+  </si>
+  <si>
+    <t>Drive-in restaurant</t>
+  </si>
+  <si>
+    <t>3-or-more story office bldg</t>
+  </si>
+  <si>
+    <t>Feed and grain mill</t>
+  </si>
+  <si>
+    <t>Indiv parcel/neighborhd shop ctr</t>
+  </si>
+  <si>
+    <t>Horse ranch w/2 or more res</t>
   </si>
   <si>
     <t>Horse ranch</t>
   </si>
   <si>
-    <t>Utility water company</t>
-  </si>
-  <si>
-    <t>Alternate use office bldgs</t>
-  </si>
-  <si>
-    <t>County building</t>
-  </si>
-  <si>
-    <t>Parochial school</t>
-  </si>
-  <si>
     <t>Winery</t>
   </si>
   <si>
-    <t>State pk/other recreation fac</t>
-  </si>
-  <si>
-    <t>Arcades &amp; amusement center</t>
+    <t>Warehousing/inactive</t>
+  </si>
+  <si>
+    <t>Mineral processing</t>
   </si>
   <si>
     <t>Service station/mini-mart</t>
   </si>
   <si>
-    <t>Sand and gravel, shale</t>
-  </si>
-  <si>
-    <t>Cocktail lounge bar</t>
-  </si>
-  <si>
-    <t>Indiv parcel/neighborhd shop ctr</t>
-  </si>
-  <si>
-    <t>Warehousing/inactive</t>
-  </si>
-  <si>
-    <t>Mineral processing</t>
+    <t>Multiple story store</t>
+  </si>
+  <si>
+    <t>Alternate use prof bldgs</t>
+  </si>
+  <si>
+    <t>State building</t>
+  </si>
+  <si>
+    <t>Alternate use service stations</t>
+  </si>
+  <si>
+    <t>Specialty shop (tires,brakes)</t>
+  </si>
+  <si>
+    <t>Assisted care facility</t>
+  </si>
+  <si>
+    <t>Auto sales w/service center</t>
+  </si>
+  <si>
+    <t>Alternate use</t>
+  </si>
+  <si>
+    <t>Cable tv</t>
+  </si>
+  <si>
+    <t>Supermarket</t>
+  </si>
+  <si>
+    <t>Volunteer fire department</t>
+  </si>
+  <si>
+    <t>Alternate use stores</t>
+  </si>
+  <si>
+    <t>Alternate use store/off combo</t>
+  </si>
+  <si>
+    <t>Sfd converted to res care fac</t>
+  </si>
+  <si>
+    <t>Horse ranch w/manufacturedhome</t>
+  </si>
+  <si>
+    <t>Self service sta/no repair facilities</t>
+  </si>
+  <si>
+    <t>Other poultry ranch</t>
+  </si>
+  <si>
+    <t>Heavy industry</t>
+  </si>
+  <si>
+    <t>Live/work units</t>
+  </si>
+  <si>
+    <t>Lumber mill</t>
+  </si>
+  <si>
+    <t>Health spa or club</t>
+  </si>
+  <si>
+    <t>Mortuary/funeral home</t>
+  </si>
+  <si>
+    <t>Multi-offices/residential units</t>
+  </si>
+  <si>
+    <t>Farm or const mach sales/serv</t>
   </si>
   <si>
     <t>Mutual water company</t>
   </si>
   <si>
-    <t>Horse ranch w/2 or more res</t>
-  </si>
-  <si>
-    <t>Multi-offices/residential units</t>
-  </si>
-  <si>
-    <t>Feed and grain mill</t>
-  </si>
-  <si>
-    <t>3-or-more story office bldg</t>
-  </si>
-  <si>
-    <t>Multiple story store</t>
-  </si>
-  <si>
-    <t>Drive-in restaurant</t>
+    <t>Dental offices</t>
+  </si>
+  <si>
+    <t>Other poultry ranch w/residence</t>
+  </si>
+  <si>
+    <t>Rural residential w/misc residential imp</t>
   </si>
   <si>
     <t>Dairy w/manufactured home</t>
   </si>
   <si>
-    <t>Heavy industry</t>
-  </si>
-  <si>
-    <t>Assisted care facility</t>
-  </si>
-  <si>
-    <t>Supermarket</t>
-  </si>
-  <si>
-    <t>Alternate use stores</t>
-  </si>
-  <si>
-    <t>Lumber mill</t>
-  </si>
-  <si>
-    <t>Alternate use store/off combo</t>
-  </si>
-  <si>
-    <t>Specialty shop (tires,brakes)</t>
-  </si>
-  <si>
-    <t>Alternate use service stations</t>
-  </si>
-  <si>
-    <t>Volunteer fire department</t>
-  </si>
-  <si>
-    <t>Alternate use prof bldgs</t>
-  </si>
-  <si>
-    <t>Live/work units</t>
-  </si>
-  <si>
-    <t>Liquor store</t>
-  </si>
-  <si>
-    <t>Alternate use</t>
-  </si>
-  <si>
-    <t>Horse ranch w/manufacturedhome</t>
-  </si>
-  <si>
-    <t>State building</t>
-  </si>
-  <si>
-    <t>Mortuary/funeral home</t>
-  </si>
-  <si>
-    <t>Health spa or club</t>
-  </si>
-  <si>
-    <t>Auto sales w/service center</t>
-  </si>
-  <si>
-    <t>Other poultry ranch w/residence</t>
+    <t>County hospital</t>
   </si>
   <si>
     <t>Radio &amp; tv broadcast site</t>
   </si>
   <si>
-    <t>Other poultry ranch</t>
-  </si>
-  <si>
     <t>Regional shopping center</t>
   </si>
   <si>
-    <t>Dental offices</t>
+    <t>Country club</t>
+  </si>
+  <si>
+    <t>Community shopping center</t>
+  </si>
+  <si>
+    <t>Retail feed and grain sales</t>
+  </si>
+  <si>
+    <t>Chicken ranch w/manufactured home</t>
+  </si>
+  <si>
+    <t>Rural res/manufactured home</t>
   </si>
   <si>
     <t>Convenience store</t>
-  </si>
-  <si>
-    <t>Community shopping center</t>
-  </si>
-  <si>
-    <t>Retail feed and grain sales</t>
-  </si>
-  <si>
-    <t>Chicken ranch w/manufactured home</t>
-  </si>
-  <si>
-    <t>Rural res/manufactured home</t>
-  </si>
-  <si>
-    <t>Farm or const mach sales/serv</t>
-  </si>
-  <si>
-    <t>Self service sta/no repair facilities</t>
-  </si>
-  <si>
-    <t>Sfd converted to res care fac</t>
-  </si>
-  <si>
-    <t>Cable tv</t>
-  </si>
-  <si>
-    <t>County hospital</t>
-  </si>
-  <si>
-    <t>Country club</t>
   </si>
 </sst>
 </file>
@@ -758,7 +749,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -803,13 +794,13 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>6</v>
       </c>
       <c r="E4">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -834,16 +825,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -851,16 +842,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E7">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -868,16 +859,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -888,13 +879,13 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -902,16 +893,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -919,16 +910,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -936,16 +927,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -956,13 +947,13 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -970,16 +961,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -987,16 +978,16 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1004,16 +995,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1021,16 +1012,16 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1038,16 +1029,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
         <v>14</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1055,13 +1046,13 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E19">
         <v>14</v>
@@ -1072,16 +1063,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1095,10 +1086,10 @@
         <v>12</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1106,16 +1097,16 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1123,16 +1114,16 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
         <v>12</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1140,16 +1131,16 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1160,10 +1151,10 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25">
         <v>12</v>
@@ -1191,16 +1182,16 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1208,16 +1199,16 @@
         <v>31</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C28">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E28">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1228,13 +1219,13 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1242,16 +1233,16 @@
         <v>33</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1276,7 +1267,7 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>9</v>
@@ -1285,7 +1276,7 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1293,16 +1284,16 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C33">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E33">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1310,13 +1301,13 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D34">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E34">
         <v>8</v>
@@ -1327,16 +1318,16 @@
         <v>38</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D35">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1344,16 +1335,16 @@
         <v>39</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1364,13 +1355,13 @@
         <v>1</v>
       </c>
       <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
         <v>6</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1395,16 +1386,16 @@
         <v>42</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1415,13 +1406,13 @@
         <v>0</v>
       </c>
       <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
         <v>5</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1432,13 +1423,13 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1446,16 +1437,16 @@
         <v>45</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1466,10 +1457,10 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43">
         <v>5</v>
@@ -1480,16 +1471,16 @@
         <v>47</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E44">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1497,7 +1488,7 @@
         <v>48</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45">
         <v>4</v>
@@ -1506,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1534,10 +1525,10 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47">
         <v>4</v>
@@ -1548,10 +1539,10 @@
         <v>51</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1565,13 +1556,13 @@
         <v>52</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E49">
         <v>4</v>
@@ -1582,13 +1573,13 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E50">
         <v>4</v>
@@ -1599,13 +1590,13 @@
         <v>54</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51">
         <v>4</v>
@@ -1616,13 +1607,13 @@
         <v>55</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E52">
         <v>4</v>
@@ -1633,13 +1624,13 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D53">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E53">
         <v>4</v>
@@ -1650,13 +1641,13 @@
         <v>57</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54">
         <v>4</v>
@@ -1667,16 +1658,16 @@
         <v>58</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1684,16 +1675,16 @@
         <v>59</v>
       </c>
       <c r="B56">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
       <c r="E56">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1704,13 +1695,13 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
       <c r="E57">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1718,16 +1709,16 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E58">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1735,10 +1726,10 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -1755,10 +1746,10 @@
         <v>0</v>
       </c>
       <c r="C60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60">
         <v>3</v>
@@ -1769,13 +1760,13 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61">
         <v>3</v>
@@ -1789,10 +1780,10 @@
         <v>0</v>
       </c>
       <c r="C62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62">
         <v>3</v>
@@ -1820,13 +1811,13 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E64">
         <v>3</v>
@@ -1888,10 +1879,10 @@
         <v>71</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -1922,16 +1913,16 @@
         <v>73</v>
       </c>
       <c r="B70">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D70">
         <v>0</v>
       </c>
       <c r="E70">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1942,13 +1933,13 @@
         <v>1</v>
       </c>
       <c r="C71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1959,13 +1950,13 @@
         <v>0</v>
       </c>
       <c r="C72">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E72">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1976,13 +1967,13 @@
         <v>0</v>
       </c>
       <c r="C73">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
       <c r="E73">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1993,10 +1984,10 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74">
         <v>2</v>
@@ -2007,13 +1998,13 @@
         <v>78</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75">
         <v>2</v>
@@ -2024,13 +2015,13 @@
         <v>79</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76">
         <v>2</v>
@@ -2041,10 +2032,10 @@
         <v>80</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2075,13 +2066,13 @@
         <v>82</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E79">
         <v>2</v>
@@ -2092,10 +2083,10 @@
         <v>83</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C80">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -2112,10 +2103,10 @@
         <v>0</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81">
         <v>2</v>
@@ -2177,10 +2168,10 @@
         <v>88</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -2197,13 +2188,13 @@
         <v>0</v>
       </c>
       <c r="C86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D86">
         <v>0</v>
       </c>
       <c r="E86">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2211,16 +2202,16 @@
         <v>90</v>
       </c>
       <c r="B87">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87">
         <v>0</v>
       </c>
       <c r="E87">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2231,13 +2222,13 @@
         <v>0</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D88">
         <v>0</v>
       </c>
       <c r="E88">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2248,13 +2239,13 @@
         <v>0</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89">
         <v>1</v>
       </c>
       <c r="E89">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2262,7 +2253,7 @@
         <v>93</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -2271,7 +2262,7 @@
         <v>0</v>
       </c>
       <c r="E90">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2279,10 +2270,10 @@
         <v>94</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -2350,10 +2341,10 @@
         <v>0</v>
       </c>
       <c r="C95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -2415,10 +2406,10 @@
         <v>102</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -2435,10 +2426,10 @@
         <v>0</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -2568,10 +2559,10 @@
         <v>111</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -2653,10 +2644,10 @@
         <v>116</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -2724,10 +2715,10 @@
         <v>0</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E117">
         <v>1</v>
@@ -2792,10 +2783,10 @@
         <v>0</v>
       </c>
       <c r="C121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E121">
         <v>1</v>
@@ -2809,63 +2800,12 @@
         <v>0</v>
       </c>
       <c r="C122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E122">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5">
-      <c r="A123" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B123">
-        <v>0</v>
-      </c>
-      <c r="C123">
-        <v>1</v>
-      </c>
-      <c r="D123">
-        <v>0</v>
-      </c>
-      <c r="E123">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5">
-      <c r="A124" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B124">
-        <v>0</v>
-      </c>
-      <c r="C124">
-        <v>1</v>
-      </c>
-      <c r="D124">
-        <v>0</v>
-      </c>
-      <c r="E124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5">
-      <c r="A125" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B125">
-        <v>0</v>
-      </c>
-      <c r="C125">
-        <v>1</v>
-      </c>
-      <c r="D125">
-        <v>0</v>
-      </c>
-      <c r="E125">
         <v>1</v>
       </c>
     </row>

</xml_diff>